<commit_message>
adjusted the status of the table
</commit_message>
<xml_diff>
--- a/Data Science Journey Tracker.xlsx
+++ b/Data Science Journey Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PA\Documents\datascience\datascience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7DFF98-B19D-42B6-9724-EFDA4BA98EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC6C2E7-D9D4-4510-B232-6F1C88A11947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4FEAEA80-D5A9-4F4F-8015-98DD1BB07A66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4FEAEA80-D5A9-4F4F-8015-98DD1BB07A66}"/>
   </bookViews>
   <sheets>
     <sheet name="Playlist" sheetId="5" r:id="rId1"/>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="E2" s="2">
         <f ca="1">POA!M3</f>
-        <v>708.5</v>
+        <v>708.49999999999977</v>
       </c>
       <c r="F2" s="2">
         <f ca="1">ROUND(E2/60,2)</f>
@@ -3775,11 +3775,11 @@
       </c>
       <c r="B3" s="11">
         <f ca="1">COUNTIF(INDIRECT("'"&amp;$A3&amp;"'!$D:$D"),B$1)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11">
         <f ca="1">SUMIF(INDIRECT("'"&amp;$A3&amp;"'!$D:$D"),B$1,INDIRECT("'"&amp;$A3&amp;"'!$C:$C"))</f>
-        <v>617.1</v>
+        <v>544.0999999999998</v>
       </c>
       <c r="D3" s="11">
         <f ca="1">COUNTIF(INDIRECT("'"&amp;$A3&amp;"'!$D:$D"),D$1)</f>
@@ -3799,19 +3799,19 @@
       </c>
       <c r="H3" s="11">
         <f ca="1">COUNTIF(INDIRECT("'"&amp;$A3&amp;"'!$D:$D"),H$1)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I3" s="11">
         <f ca="1">SUMIF(INDIRECT("'"&amp;$A3&amp;"'!$D:$D"),H$1,INDIRECT("'"&amp;$A3&amp;"'!$C:$C"))</f>
-        <v>91.4</v>
+        <v>164.4</v>
       </c>
       <c r="J3" s="11">
         <f t="shared" ref="J3:J11" ca="1" si="0">SUM(B3,D3)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K3" s="11">
         <f t="shared" ref="K3:K11" ca="1" si="1">SUM(C3,E3)</f>
-        <v>617.1</v>
+        <v>544.0999999999998</v>
       </c>
       <c r="L3" s="11">
         <f t="shared" ref="L3:L8" ca="1" si="2">SUM(B3,D3,F3,H3)</f>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="M3" s="11">
         <f t="shared" ref="M3:M11" ca="1" si="3">SUM(C3,E3,I3)</f>
-        <v>708.5</v>
+        <v>708.49999999999977</v>
       </c>
       <c r="N3" s="11">
         <f ca="1">ROUND(M3/60,2)</f>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="O3" s="11">
         <f t="shared" ref="O3:O8" ca="1" si="4">ROUND(((H3+F3)/L3)*100,2)</f>
-        <v>9.6199999999999992</v>
+        <v>15.38</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4332,11 +4332,11 @@
       </c>
       <c r="B12" s="8">
         <f ca="1">SUM(B3:B11)</f>
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C12" s="8">
         <f t="shared" ref="C12:N12" ca="1" si="16">SUM(C3:C11)</f>
-        <v>8442.9</v>
+        <v>8369.8999999999978</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" ca="1" si="16"/>
@@ -4356,19 +4356,19 @@
       </c>
       <c r="H12" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I12" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>91.4</v>
+        <v>164.4</v>
       </c>
       <c r="J12" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>8442.9</v>
+        <v>8369.8999999999978</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" ca="1" si="16"/>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="O12" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v>1.1299999999999999</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4549,7 +4549,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4706,7 +4706,7 @@
         <v>26.7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
         <v>405</v>
@@ -4726,7 +4726,7 @@
         <v>16.8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
         <v>405</v>
@@ -4746,7 +4746,7 @@
         <v>29.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E10" t="s">
         <v>405</v>
@@ -5580,7 +5580,7 @@
       </c>
       <c r="D55" s="1">
         <f>COUNTIF(Python!D3:D54,Playlist!$I$5)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -6082,7 +6082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3FFC70-AEF8-4F32-A6C4-A57890A18299}">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>